<commit_message>
fix javascript bugs for blog rating
</commit_message>
<xml_diff>
--- a/_document/Checklist-end.xlsx
+++ b/_document/Checklist-end.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>STT</t>
   </si>
@@ -87,16 +87,19 @@
     <t>30.000.000 VND</t>
   </si>
   <si>
-    <t>Release</t>
-  </si>
-  <si>
     <t>Document source, wiki…</t>
   </si>
   <si>
     <t>Deploy, Fix bugs</t>
   </si>
   <si>
-    <t>Fix bug</t>
+    <t>Fix bug 1</t>
+  </si>
+  <si>
+    <t>Fix bug 2</t>
+  </si>
+  <si>
+    <t>Logo widget on Homepage</t>
   </si>
 </sst>
 </file>
@@ -225,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -259,6 +262,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,10 +569,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A7:S24"/>
+  <dimension ref="A7:XFD24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -646,7 +650,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="20"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -669,7 +673,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="20"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -692,7 +696,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
-      <c r="J10" s="2"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -715,7 +719,7 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="2"/>
+      <c r="J11" s="20"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -738,8 +742,8 @@
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -761,7 +765,7 @@
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
+      <c r="J13" s="20"/>
       <c r="K13" s="15"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -774,7 +778,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="12" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>5</v>
@@ -784,7 +788,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="10"/>
+      <c r="J14" s="20"/>
       <c r="K14" s="10"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -807,7 +811,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="11"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="11"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -830,14 +834,14 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19 16384:16384">
       <c r="A17" s="2">
         <v>10</v>
       </c>
@@ -853,14 +857,14 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="J17" s="20"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19 16384:16384">
       <c r="A18" s="6">
         <v>11</v>
       </c>
@@ -876,20 +880,21 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="J18" s="20"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="11"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="1:19">
+      <c r="XFD18" s="11"/>
+    </row>
+    <row r="19" spans="1:19 16384:16384">
       <c r="A19" s="6">
         <v>12</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>5</v>
@@ -899,14 +904,14 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="J19" s="20"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="10"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19 16384:16384">
       <c r="A20" s="6">
         <v>13</v>
       </c>
@@ -922,14 +927,14 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="J20" s="20"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
+      <c r="M20" s="10"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19 16384:16384">
       <c r="A21" s="5">
         <v>14</v>
       </c>
@@ -945,20 +950,20 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="J21" s="20"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="5"/>
       <c r="N21" s="2"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19 16384:16384">
       <c r="A22" s="6">
         <v>15</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>19</v>
@@ -968,18 +973,21 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="J22" s="20"/>
       <c r="K22" s="2"/>
       <c r="L22" s="11"/>
       <c r="M22" s="2"/>
       <c r="N22" s="11"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:19" ht="21">
+    <row r="23" spans="1:19 16384:16384" ht="21">
+      <c r="C23" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="L23" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="N23" t="s">
+        <v>25</v>
+      </c>
+      <c r="N23" s="16" t="s">
         <v>26</v>
       </c>
       <c r="P23" s="17" t="s">
@@ -989,7 +997,7 @@
       <c r="R23" s="17"/>
       <c r="S23" s="17"/>
     </row>
-    <row r="24" spans="1:19" ht="21">
+    <row r="24" spans="1:19 16384:16384" ht="21">
       <c r="P24" s="17" t="s">
         <v>22</v>
       </c>

</xml_diff>